<commit_message>
Moved supply RC policy mapping out of the SupplyDemand.xlsx file so that we don't have to copy the worksheet into each new version of SupplyDemand.
</commit_message>
<xml_diff>
--- a/resources/SupplyDemand.xlsx
+++ b/resources/SupplyDemand.xlsx
@@ -5,12 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SupplyDemand" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SRC_By_Day" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="policy_map" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="644">
   <si>
     <t xml:space="preserve">SRC2</t>
   </si>
@@ -1966,12 +1965,6 @@
   </si>
   <si>
     <t xml:space="preserve">Total Army Strength</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CompositePolicyName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAA_2125_R2_RC</t>
   </si>
 </sst>
 </file>
@@ -1981,7 +1974,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2009,12 +2002,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2059,17 +2046,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2095,7 +2078,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.27"/>
@@ -20729,11 +20712,11 @@
   </sheetPr>
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.55"/>
@@ -20976,47 +20959,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.33"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>645</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>